<commit_message>
Used Calamine for reading files. Added dependencies. Changed app.py to use the new reader. Changed test for the reader. Added Test for the Writer.
</commit_message>
<xml_diff>
--- a/test_data/excel_reader_test_0.xlsx
+++ b/test_data/excel_reader_test_0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benedek\Nextcloud\Uni\BP\GroupGen\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Python\GroupGen\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0596B11-F3AB-4BA6-9A08-F32EE8E8C7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4091CD08-64C8-4A9D-A368-E7DFA70735F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" xr2:uid="{F85225F5-FB8C-4177-9C2D-EFF4F79F0829}"/>
+    <workbookView xWindow="38280" yWindow="1635" windowWidth="29040" windowHeight="15720" xr2:uid="{F85225F5-FB8C-4177-9C2D-EFF4F79F0829}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -119,9 +108,6 @@
     <t>H</t>
   </si>
   <si>
-    <t>I</t>
-  </si>
-  <si>
     <t>J</t>
   </si>
   <si>
@@ -129,6 +115,9 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>49000011122.56</t>
   </si>
 </sst>
 </file>
@@ -173,13 +162,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -514,11 +504,12 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -588,8 +579,8 @@
       <c r="I2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J2">
-        <v>49000011122</v>
+      <c r="J2" t="s">
+        <v>30</v>
       </c>
       <c r="K2" t="s">
         <v>20</v>
@@ -623,17 +614,17 @@
       <c r="H3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="2">
+        <v>43968</v>
+      </c>
+      <c r="J3" t="s">
         <v>27</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>28</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>29</v>
-      </c>
-      <c r="L3" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
empty columns ignored on read, empty columns added to test data
</commit_message>
<xml_diff>
--- a/test_data/excel_reader_test_0.xlsx
+++ b/test_data/excel_reader_test_0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Python\GroupGen\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desktop_Ordner\Studium\5._Semester\BP\GroupGen\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4091CD08-64C8-4A9D-A368-E7DFA70735F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9748072A-C5AD-43C3-81B9-74132AA26809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="1635" windowWidth="29040" windowHeight="15720" xr2:uid="{F85225F5-FB8C-4177-9C2D-EFF4F79F0829}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F85225F5-FB8C-4177-9C2D-EFF4F79F0829}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Angemeldet</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>49000011122.56</t>
+  </si>
+  <si>
+    <t>Empty Column 1</t>
+  </si>
+  <si>
+    <t>Empty Column 2</t>
   </si>
 </sst>
 </file>
@@ -168,8 +174,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -501,19 +507,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C20BA79-E736-4525-8539-319E0CBE8E92}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,31 +533,37 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -564,32 +576,32 @@
       <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>4444</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>30</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>20</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -602,34 +614,34 @@
       <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>43968</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>27</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>28</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{3E33AF65-1668-4B10-998D-75D40C0C872F}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{3E33AF65-1668-4B10-998D-75D40C0C872F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
58 - empty columns ignored (#121)
empty columns ignored on read, empty columns added to test data
</commit_message>
<xml_diff>
--- a/test_data/excel_reader_test_0.xlsx
+++ b/test_data/excel_reader_test_0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Python\GroupGen\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desktop_Ordner\Studium\5._Semester\BP\GroupGen\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4091CD08-64C8-4A9D-A368-E7DFA70735F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9748072A-C5AD-43C3-81B9-74132AA26809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="1635" windowWidth="29040" windowHeight="15720" xr2:uid="{F85225F5-FB8C-4177-9C2D-EFF4F79F0829}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F85225F5-FB8C-4177-9C2D-EFF4F79F0829}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Angemeldet</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>49000011122.56</t>
+  </si>
+  <si>
+    <t>Empty Column 1</t>
+  </si>
+  <si>
+    <t>Empty Column 2</t>
   </si>
 </sst>
 </file>
@@ -168,8 +174,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -501,19 +507,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C20BA79-E736-4525-8539-319E0CBE8E92}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,31 +533,37 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -564,32 +576,32 @@
       <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>4444</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>30</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>20</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -602,34 +614,34 @@
       <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>43968</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>27</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>28</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{3E33AF65-1668-4B10-998D-75D40C0C872F}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{3E33AF65-1668-4B10-998D-75D40C0C872F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>